<commit_message>
done a coef frame
</commit_message>
<xml_diff>
--- a/months/dec22test/dec22.xlsx
+++ b/months/dec22test/dec22.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="таблица на холод" sheetId="1" state="visible" r:id="rId2"/>
@@ -497,7 +497,7 @@
     <t xml:space="preserve">SUM</t>
   </si>
   <si>
-    <t xml:space="preserve">duty_24</t>
+    <t xml:space="preserve">dutyTrue</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;.22: 3*, &lt;.23: 2*, &gt;=.23: 0</t>
@@ -524,7 +524,7 @@
     <t xml:space="preserve">20*</t>
   </si>
   <si>
-    <t xml:space="preserve">duty_False</t>
+    <t xml:space="preserve">dutyFalse</t>
   </si>
   <si>
     <t xml:space="preserve">True</t>
@@ -545,7 +545,7 @@
     <t xml:space="preserve">False</t>
   </si>
   <si>
-    <t xml:space="preserve">duty_8</t>
+    <t xml:space="preserve">duty8</t>
   </si>
   <si>
     <t xml:space="preserve">WEAK1</t>
@@ -759,7 +759,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="44">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -885,10 +885,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1106,12 +1102,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="6.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="5.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="7.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="7.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="6.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="5.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="5.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="2" width="6.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="5.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="2" width="6.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="2" width="5.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="2" width="5.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="4" width="18"/>
@@ -2772,11 +2768,11 @@
   </sheetPr>
   <dimension ref="A1:AD34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="6.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="30" width="4.43"/>
@@ -2794,7 +2790,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="7.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="11.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="6.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="20" style="0" width="7.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="20" style="0" width="7.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="11.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="6.28"/>
   </cols>
@@ -4918,13 +4914,12 @@
       <selection pane="topLeft" activeCell="J8" activeCellId="0" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="31" width="13.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="31" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="32" width="5.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="5.43"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="4" style="31" width="8.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="6" style="32" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4935,7 +4930,7 @@
       <c r="B1" s="31" t="s">
         <v>148</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="0" t="s">
         <v>149</v>
       </c>
       <c r="D1" s="31" t="s">
@@ -4944,10 +4939,10 @@
       <c r="E1" s="31" t="s">
         <v>151</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="0" t="s">
         <v>152</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="G1" s="0" t="s">
         <v>153</v>
       </c>
     </row>
@@ -4960,18 +4955,18 @@
         <f aca="false">IFERROR(IF(FIND(":",A2)&gt;0,"long_box"),"fine/enc")</f>
         <v>long_box</v>
       </c>
-      <c r="C2" s="32" t="n">
+      <c r="C2" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="D2" s="32" t="n">
+      <c r="D2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32" t="n">
+      <c r="E2" s="0"/>
+      <c r="F2" s="0" t="n">
         <f aca="false">IF(D2="",,C2*D2)</f>
         <v>100</v>
       </c>
-      <c r="G2" s="32" t="n">
+      <c r="G2" s="0" t="n">
         <f aca="false">IF(E2="",,C2*E2)</f>
         <v>0</v>
       </c>
@@ -4985,20 +4980,20 @@
         <f aca="false">IFERROR(IF(FIND(":",A3)&gt;0,"long_box"),"fine/enc")</f>
         <v>long_box</v>
       </c>
-      <c r="C3" s="32" t="n">
+      <c r="C3" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="D3" s="32" t="n">
+      <c r="D3" s="0" t="n">
         <v>0.5</v>
       </c>
-      <c r="E3" s="32" t="n">
+      <c r="E3" s="0" t="n">
         <v>0.5</v>
       </c>
-      <c r="F3" s="32" t="n">
+      <c r="F3" s="0" t="n">
         <f aca="false">IF(D3="",,C3*D3)</f>
         <v>50</v>
       </c>
-      <c r="G3" s="32" t="n">
+      <c r="G3" s="0" t="n">
         <f aca="false">IF(E3="",,C3*E3)</f>
         <v>50</v>
       </c>
@@ -5012,20 +5007,20 @@
         <f aca="false">IFERROR(IF(FIND(":",A4)&gt;0,"long_box"),"fine/enc")</f>
         <v>long_box</v>
       </c>
-      <c r="C4" s="32" t="n">
+      <c r="C4" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="D4" s="32" t="n">
+      <c r="D4" s="0" t="n">
         <v>0.5</v>
       </c>
-      <c r="E4" s="32" t="n">
+      <c r="E4" s="0" t="n">
         <v>0.5</v>
       </c>
-      <c r="F4" s="32" t="n">
+      <c r="F4" s="0" t="n">
         <f aca="false">IF(D4="",,C4*D4)</f>
         <v>50</v>
       </c>
-      <c r="G4" s="32" t="n">
+      <c r="G4" s="0" t="n">
         <f aca="false">IF(E4="",,C4*E4)</f>
         <v>50</v>
       </c>
@@ -5039,18 +5034,18 @@
         <f aca="false">IFERROR(IF(FIND(":",A5)&gt;0,"long_box"),"fine/enc")</f>
         <v>long_box</v>
       </c>
-      <c r="C5" s="32" t="n">
+      <c r="C5" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="D5" s="32" t="n">
+      <c r="D5" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32" t="n">
+      <c r="E5" s="0"/>
+      <c r="F5" s="0" t="n">
         <f aca="false">IF(D5="",,C5*D5)</f>
         <v>100</v>
       </c>
-      <c r="G5" s="32" t="n">
+      <c r="G5" s="0" t="n">
         <f aca="false">IF(E5="",,C5*E5)</f>
         <v>0</v>
       </c>
@@ -5064,18 +5059,18 @@
         <f aca="false">IFERROR(IF(FIND(":",A6)&gt;0,"long_box"),"fine/enc")</f>
         <v>long_box</v>
       </c>
-      <c r="C6" s="32" t="n">
+      <c r="C6" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32" t="n">
+      <c r="D6" s="0"/>
+      <c r="E6" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F6" s="32" t="n">
+      <c r="F6" s="0" t="n">
         <f aca="false">IF(D6="",,C6*D6)</f>
         <v>0</v>
       </c>
-      <c r="G6" s="32" t="n">
+      <c r="G6" s="0" t="n">
         <f aca="false">IF(E6="",,C6*E6)</f>
         <v>100</v>
       </c>
@@ -5089,18 +5084,18 @@
         <f aca="false">IFERROR(IF(FIND(":",A7)&gt;0,"long_box"),"fine/enc")</f>
         <v>long_box</v>
       </c>
-      <c r="C7" s="32" t="n">
+      <c r="C7" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="D7" s="32" t="n">
+      <c r="D7" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32" t="n">
+      <c r="E7" s="0"/>
+      <c r="F7" s="0" t="n">
         <f aca="false">IF(D7="",,C7*D7)</f>
         <v>100</v>
       </c>
-      <c r="G7" s="32" t="n">
+      <c r="G7" s="0" t="n">
         <f aca="false">IF(E7="",,C7*E7)</f>
         <v>0</v>
       </c>
@@ -5114,18 +5109,18 @@
         <f aca="false">IFERROR(IF(FIND(":",A8)&gt;0,"long_box"),"fine/enc")</f>
         <v>long_box</v>
       </c>
-      <c r="C8" s="32" t="n">
+      <c r="C8" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="D8" s="32" t="n">
+      <c r="D8" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E8" s="32"/>
-      <c r="F8" s="32" t="n">
+      <c r="E8" s="0"/>
+      <c r="F8" s="0" t="n">
         <f aca="false">IF(D8="",,C8*D8)</f>
         <v>100</v>
       </c>
-      <c r="G8" s="32" t="n">
+      <c r="G8" s="0" t="n">
         <f aca="false">IF(E8="",,C8*E8)</f>
         <v>0</v>
       </c>
@@ -5139,18 +5134,18 @@
         <f aca="false">IFERROR(IF(FIND(":",A9)&gt;0,"long_box"),"fine/enc")</f>
         <v>long_box</v>
       </c>
-      <c r="C9" s="32" t="n">
+      <c r="C9" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="D9" s="32" t="n">
+      <c r="D9" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32" t="n">
+      <c r="E9" s="0"/>
+      <c r="F9" s="0" t="n">
         <f aca="false">IF(D9="",,C9*D9)</f>
         <v>100</v>
       </c>
-      <c r="G9" s="32" t="n">
+      <c r="G9" s="0" t="n">
         <f aca="false">IF(E9="",,C9*E9)</f>
         <v>0</v>
       </c>
@@ -5164,13 +5159,13 @@
         <f aca="false">IFERROR(IF(FIND(":",A10)&gt;0,"long_box"),"fine/enc")</f>
         <v>fine/enc</v>
       </c>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32" t="n">
+      <c r="D10" s="0"/>
+      <c r="E10" s="0"/>
+      <c r="F10" s="0" t="n">
         <f aca="false">IF(D10="",,C10*D10)</f>
         <v>0</v>
       </c>
-      <c r="G10" s="32" t="n">
+      <c r="G10" s="0" t="n">
         <f aca="false">IF(E10="",,C10*E10)</f>
         <v>0</v>
       </c>
@@ -5184,13 +5179,13 @@
         <f aca="false">IFERROR(IF(FIND(":",A11)&gt;0,"long_box"),"fine/enc")</f>
         <v>fine/enc</v>
       </c>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32" t="n">
+      <c r="D11" s="0"/>
+      <c r="E11" s="0"/>
+      <c r="F11" s="0" t="n">
         <f aca="false">IF(D11="",,C11*D11)</f>
         <v>0</v>
       </c>
-      <c r="G11" s="32" t="n">
+      <c r="G11" s="0" t="n">
         <f aca="false">IF(E11="",,C11*E11)</f>
         <v>0</v>
       </c>
@@ -5204,13 +5199,13 @@
         <f aca="false">IFERROR(IF(FIND(":",A12)&gt;0,"long_box"),"fine/enc")</f>
         <v>fine/enc</v>
       </c>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32" t="n">
+      <c r="D12" s="0"/>
+      <c r="E12" s="0"/>
+      <c r="F12" s="0" t="n">
         <f aca="false">IF(D12="",,C12*D12)</f>
         <v>0</v>
       </c>
-      <c r="G12" s="32" t="n">
+      <c r="G12" s="0" t="n">
         <f aca="false">IF(E12="",,C12*E12)</f>
         <v>0</v>
       </c>
@@ -5224,13 +5219,13 @@
         <f aca="false">IFERROR(IF(FIND(":",A13)&gt;0,"long_box"),"fine/enc")</f>
         <v>fine/enc</v>
       </c>
-      <c r="D13" s="32"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32" t="n">
+      <c r="D13" s="0"/>
+      <c r="E13" s="0"/>
+      <c r="F13" s="0" t="n">
         <f aca="false">IF(D13="",,C13*D13)</f>
         <v>0</v>
       </c>
-      <c r="G13" s="32" t="n">
+      <c r="G13" s="0" t="n">
         <f aca="false">IF(E13="",,C13*E13)</f>
         <v>0</v>
       </c>
@@ -5244,13 +5239,13 @@
         <f aca="false">IFERROR(IF(FIND(":",A14)&gt;0,"long_box"),"fine/enc")</f>
         <v>fine/enc</v>
       </c>
-      <c r="D14" s="32"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="32" t="n">
+      <c r="D14" s="0"/>
+      <c r="E14" s="0"/>
+      <c r="F14" s="0" t="n">
         <f aca="false">IF(D14="",,C14*D14)</f>
         <v>0</v>
       </c>
-      <c r="G14" s="32" t="n">
+      <c r="G14" s="0" t="n">
         <f aca="false">IF(E14="",,C14*E14)</f>
         <v>0</v>
       </c>
@@ -5264,13 +5259,13 @@
         <f aca="false">IFERROR(IF(FIND(":",A15)&gt;0,"long_box"),"fine/enc")</f>
         <v>fine/enc</v>
       </c>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32" t="n">
+      <c r="D15" s="0"/>
+      <c r="E15" s="0"/>
+      <c r="F15" s="0" t="n">
         <f aca="false">IF(D15="",,C15*D15)</f>
         <v>0</v>
       </c>
-      <c r="G15" s="32" t="n">
+      <c r="G15" s="0" t="n">
         <f aca="false">IF(E15="",,C15*E15)</f>
         <v>0</v>
       </c>
@@ -5284,20 +5279,20 @@
         <f aca="false">IFERROR(IF(FIND(":",A16)&gt;0,"long_box"),"fine/enc")</f>
         <v>fine/enc</v>
       </c>
-      <c r="C16" s="32" t="n">
+      <c r="C16" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="D16" s="32" t="s">
+      <c r="D16" s="0" t="s">
         <v>154</v>
       </c>
-      <c r="E16" s="32" t="s">
+      <c r="E16" s="0" t="s">
         <v>104</v>
       </c>
-      <c r="F16" s="32" t="n">
+      <c r="F16" s="0" t="n">
         <f aca="false">IF(D16="",,C16*D16)</f>
         <v>450</v>
       </c>
-      <c r="G16" s="32" t="n">
+      <c r="G16" s="0" t="n">
         <f aca="false">IF(E16="",,C16*E16)</f>
         <v>200</v>
       </c>
@@ -5311,13 +5306,13 @@
         <f aca="false">IFERROR(IF(FIND(":",A17)&gt;0,"long_box"),"fine/enc")</f>
         <v>fine/enc</v>
       </c>
-      <c r="D17" s="32"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32" t="n">
+      <c r="D17" s="0"/>
+      <c r="E17" s="0"/>
+      <c r="F17" s="0" t="n">
         <f aca="false">IF(D17="",,C17*D17)</f>
         <v>0</v>
       </c>
-      <c r="G17" s="32" t="n">
+      <c r="G17" s="0" t="n">
         <f aca="false">IF(E17="",,C17*E17)</f>
         <v>0</v>
       </c>
@@ -5331,13 +5326,13 @@
         <f aca="false">IFERROR(IF(FIND(":",A18)&gt;0,"long_box"),"fine/enc")</f>
         <v>fine/enc</v>
       </c>
-      <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32" t="n">
+      <c r="D18" s="0"/>
+      <c r="E18" s="0"/>
+      <c r="F18" s="0" t="n">
         <f aca="false">IF(D18="",,C18*D18)</f>
         <v>0</v>
       </c>
-      <c r="G18" s="32" t="n">
+      <c r="G18" s="0" t="n">
         <f aca="false">IF(E18="",,C18*E18)</f>
         <v>0</v>
       </c>
@@ -5351,13 +5346,13 @@
         <f aca="false">IFERROR(IF(FIND(":",A19)&gt;0,"long_box"),"fine/enc")</f>
         <v>fine/enc</v>
       </c>
-      <c r="D19" s="32"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="32" t="n">
+      <c r="D19" s="0"/>
+      <c r="E19" s="0"/>
+      <c r="F19" s="0" t="n">
         <f aca="false">IF(D19="",,C19*D19)</f>
         <v>0</v>
       </c>
-      <c r="G19" s="32" t="n">
+      <c r="G19" s="0" t="n">
         <f aca="false">IF(E19="",,C19*E19)</f>
         <v>0</v>
       </c>
@@ -5371,16 +5366,16 @@
         <f aca="false">IFERROR(IF(FIND(":",A20)&gt;0,"long_box"),"fine/enc")</f>
         <v>fine/enc</v>
       </c>
-      <c r="C20" s="32" t="n">
+      <c r="C20" s="0" t="n">
         <v>-100</v>
       </c>
-      <c r="D20" s="32"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="32" t="n">
+      <c r="D20" s="0"/>
+      <c r="E20" s="0"/>
+      <c r="F20" s="0" t="n">
         <f aca="false">IF(D20="",,C20*D20)</f>
         <v>0</v>
       </c>
-      <c r="G20" s="32" t="n">
+      <c r="G20" s="0" t="n">
         <f aca="false">IF(E20="",,C20*E20)</f>
         <v>0</v>
       </c>
@@ -5394,16 +5389,16 @@
         <f aca="false">IFERROR(IF(FIND(":",A21)&gt;0,"long_box"),"fine/enc")</f>
         <v>fine/enc</v>
       </c>
-      <c r="C21" s="32" t="n">
+      <c r="C21" s="0" t="n">
         <v>-100</v>
       </c>
-      <c r="D21" s="32"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="32" t="n">
+      <c r="D21" s="0"/>
+      <c r="E21" s="0"/>
+      <c r="F21" s="0" t="n">
         <f aca="false">IF(D21="",,C21*D21)</f>
         <v>0</v>
       </c>
-      <c r="G21" s="32" t="n">
+      <c r="G21" s="0" t="n">
         <f aca="false">IF(E21="",,C21*E21)</f>
         <v>0</v>
       </c>
@@ -5417,20 +5412,20 @@
         <f aca="false">IFERROR(IF(FIND(":",A22)&gt;0,"long_box"),"fine/enc")</f>
         <v>fine/enc</v>
       </c>
-      <c r="C22" s="32" t="n">
+      <c r="C22" s="0" t="n">
         <v>-50</v>
       </c>
-      <c r="D22" s="32" t="n">
+      <c r="D22" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="E22" s="32" t="n">
+      <c r="E22" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="F22" s="32" t="n">
+      <c r="F22" s="0" t="n">
         <f aca="false">IF(D22="",,C22*D22)</f>
         <v>-350</v>
       </c>
-      <c r="G22" s="32" t="n">
+      <c r="G22" s="0" t="n">
         <f aca="false">IF(E22="",,C22*E22)</f>
         <v>-200</v>
       </c>
@@ -5444,20 +5439,20 @@
         <f aca="false">IFERROR(IF(FIND(":",A23)&gt;0,"long_box"),"fine/enc")</f>
         <v>fine/enc</v>
       </c>
-      <c r="C23" s="32" t="n">
+      <c r="C23" s="0" t="n">
         <v>-100</v>
       </c>
-      <c r="D23" s="32" t="n">
+      <c r="D23" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="E23" s="32" t="n">
+      <c r="E23" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F23" s="32" t="n">
+      <c r="F23" s="0" t="n">
         <f aca="false">IF(D23="",,C23*D23)</f>
         <v>-200</v>
       </c>
-      <c r="G23" s="32" t="n">
+      <c r="G23" s="0" t="n">
         <f aca="false">IF(E23="",,C23*E23)</f>
         <v>-100</v>
       </c>
@@ -5471,18 +5466,18 @@
         <f aca="false">IFERROR(IF(FIND(":",A24)&gt;0,"long_box"),"fine/enc")</f>
         <v>fine/enc</v>
       </c>
-      <c r="C24" s="32" t="n">
+      <c r="C24" s="0" t="n">
         <v>-100</v>
       </c>
-      <c r="D24" s="32" t="n">
+      <c r="D24" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="E24" s="32"/>
-      <c r="F24" s="32" t="n">
+      <c r="E24" s="0"/>
+      <c r="F24" s="0" t="n">
         <f aca="false">IF(D24="",,C24*D24)</f>
         <v>-200</v>
       </c>
-      <c r="G24" s="32" t="n">
+      <c r="G24" s="0" t="n">
         <f aca="false">IF(E24="",,C24*E24)</f>
         <v>0</v>
       </c>
@@ -5496,16 +5491,16 @@
         <f aca="false">IFERROR(IF(FIND(":",A25)&gt;0,"long_box"),"fine/enc")</f>
         <v>fine/enc</v>
       </c>
-      <c r="C25" s="32" t="n">
+      <c r="C25" s="0" t="n">
         <v>-100</v>
       </c>
-      <c r="D25" s="32"/>
-      <c r="E25" s="32"/>
-      <c r="F25" s="32" t="n">
+      <c r="D25" s="0"/>
+      <c r="E25" s="0"/>
+      <c r="F25" s="0" t="n">
         <f aca="false">IF(D25="",,C25*D25)</f>
         <v>0</v>
       </c>
-      <c r="G25" s="32" t="n">
+      <c r="G25" s="0" t="n">
         <f aca="false">IF(E25="",,C25*E25)</f>
         <v>0</v>
       </c>
@@ -5519,18 +5514,18 @@
         <f aca="false">IFERROR(IF(FIND(":",A26)&gt;0,"long_box"),"fine/enc")</f>
         <v>fine/enc</v>
       </c>
-      <c r="C26" s="32" t="n">
+      <c r="C26" s="0" t="n">
         <v>-100</v>
       </c>
-      <c r="D26" s="32" t="n">
+      <c r="D26" s="0" t="n">
         <v>-4</v>
       </c>
-      <c r="E26" s="32"/>
-      <c r="F26" s="32" t="n">
+      <c r="E26" s="0"/>
+      <c r="F26" s="0" t="n">
         <f aca="false">IF(D26="",,C26*D26)</f>
         <v>400</v>
       </c>
-      <c r="G26" s="32" t="n">
+      <c r="G26" s="0" t="n">
         <f aca="false">IF(E26="",,C26*E26)</f>
         <v>0</v>
       </c>
@@ -5544,35 +5539,35 @@
         <f aca="false">IFERROR(IF(FIND(":",A27)&gt;0,"long_box"),"fine/enc")</f>
         <v>fine/enc</v>
       </c>
-      <c r="C27" s="32" t="n">
+      <c r="C27" s="0" t="n">
         <v>-100</v>
       </c>
-      <c r="D27" s="32" t="n">
+      <c r="D27" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E27" s="32"/>
-      <c r="F27" s="32" t="n">
+      <c r="E27" s="0"/>
+      <c r="F27" s="0" t="n">
         <f aca="false">IF(D27="",,C27*D27)</f>
         <v>-100</v>
       </c>
-      <c r="G27" s="32" t="n">
+      <c r="G27" s="0" t="n">
         <f aca="false">IF(E27="",,C27*E27)</f>
         <v>0</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="33" t="s">
+      <c r="A28" s="32" t="s">
         <v>155</v>
       </c>
-      <c r="B28" s="33"/>
-      <c r="C28" s="34"/>
-      <c r="D28" s="33"/>
-      <c r="E28" s="33"/>
-      <c r="F28" s="34" t="n">
+      <c r="B28" s="32"/>
+      <c r="C28" s="33"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="33" t="n">
         <f aca="false">SUM(F2:F27)</f>
         <v>600</v>
       </c>
-      <c r="G28" s="34" t="n">
+      <c r="G28" s="33" t="n">
         <f aca="false">SUM(G2:G27)</f>
         <v>100</v>
       </c>
@@ -5595,758 +5590,758 @@
   </sheetPr>
   <dimension ref="A1:U11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G22" activeCellId="0" sqref="G22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="7.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="35" width="7.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="7.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="34" width="7.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="10.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="4.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="4.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="6.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="7.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="22.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="6.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="7.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="7.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="22.85"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="35" t="s">
         <v>149</v>
       </c>
-      <c r="B1" s="37" t="str">
+      <c r="B1" s="36" t="str">
         <f aca="false">vedomost!F1</f>
         <v>A:GYM</v>
       </c>
-      <c r="C1" s="37" t="str">
+      <c r="C1" s="36" t="str">
         <f aca="false">vedomost!G1</f>
         <v>A:SLEEPTIME</v>
       </c>
-      <c r="D1" s="37" t="str">
+      <c r="D1" s="36" t="str">
         <f aca="false">vedomost!H1</f>
         <v>Z:STROLL</v>
       </c>
-      <c r="E1" s="37" t="str">
+      <c r="E1" s="36" t="str">
         <f aca="false">vedomost!I1</f>
         <v>Z:SLEEPTIME</v>
       </c>
-      <c r="F1" s="37" t="str">
+      <c r="F1" s="36" t="str">
         <f aca="false">vedomost!J1</f>
         <v>Z:TEETH</v>
       </c>
-      <c r="G1" s="37" t="str">
+      <c r="G1" s="36" t="str">
         <f aca="false">vedomost!K1</f>
         <v>Z:TELE</v>
       </c>
-      <c r="H1" s="37" t="str">
+      <c r="H1" s="36" t="str">
         <f aca="false">vedomost!L1</f>
         <v>F:VACUUM</v>
       </c>
-      <c r="I1" s="37" t="str">
+      <c r="I1" s="36" t="str">
         <f aca="false">vedomost!M1</f>
         <v>F:KITCHEN</v>
       </c>
-      <c r="J1" s="37" t="str">
+      <c r="J1" s="36" t="str">
         <f aca="false">vedomost!N1</f>
         <v>E:HYGIENE</v>
       </c>
-      <c r="K1" s="37" t="str">
+      <c r="K1" s="36" t="str">
         <f aca="false">vedomost!O1</f>
         <v>E:PY</v>
       </c>
-      <c r="L1" s="37" t="str">
+      <c r="L1" s="36" t="str">
         <f aca="false">vedomost!P1</f>
         <v>E:VIM</v>
       </c>
-      <c r="M1" s="37" t="str">
+      <c r="M1" s="36" t="str">
         <f aca="false">vedomost!Q1</f>
         <v>E:PLAN</v>
       </c>
-      <c r="N1" s="37" t="str">
+      <c r="N1" s="36" t="str">
         <f aca="false">vedomost!R1</f>
         <v>E:SLEEPTIME</v>
       </c>
-      <c r="O1" s="37" t="str">
+      <c r="O1" s="36" t="str">
         <f aca="false">vedomost!S1</f>
         <v>E:DIET</v>
       </c>
-      <c r="P1" s="37" t="str">
+      <c r="P1" s="36" t="str">
         <f aca="false">vedomost!T1</f>
         <v>E:MEALS</v>
       </c>
-      <c r="Q1" s="37" t="str">
+      <c r="Q1" s="36" t="str">
         <f aca="false">vedomost!U1</f>
         <v>L:TEETH</v>
       </c>
-      <c r="R1" s="37" t="str">
+      <c r="R1" s="36" t="str">
         <f aca="false">vedomost!V1</f>
         <v>L:SLEEPTIME</v>
       </c>
-      <c r="S1" s="37" t="str">
+      <c r="S1" s="36" t="str">
         <f aca="false">vedomost!W1</f>
         <v>L:DIET</v>
       </c>
-      <c r="T1" s="37" t="str">
+      <c r="T1" s="36" t="str">
         <f aca="false">vedomost!X1</f>
         <v>L:MEALS</v>
       </c>
-      <c r="U1" s="37" t="str">
+      <c r="U1" s="36" t="str">
         <f aca="false">vedomost!Y1</f>
         <v>L:ALARM</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="37" t="s">
         <v>156</v>
       </c>
-      <c r="B2" s="37" t="n">
+      <c r="B2" s="36" t="n">
         <v>100</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="36" t="s">
         <v>157</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="36" t="s">
         <v>158</v>
       </c>
-      <c r="E2" s="37" t="s">
+      <c r="E2" s="36" t="s">
         <v>157</v>
       </c>
-      <c r="F2" s="37" t="n">
+      <c r="F2" s="36" t="n">
         <v>50</v>
       </c>
-      <c r="G2" s="37" t="n">
+      <c r="G2" s="36" t="n">
         <v>300</v>
       </c>
-      <c r="H2" s="37" t="s">
+      <c r="H2" s="36" t="s">
         <v>159</v>
       </c>
-      <c r="I2" s="37" t="n">
+      <c r="I2" s="36" t="n">
         <v>100</v>
       </c>
-      <c r="J2" s="37" t="n">
+      <c r="J2" s="36" t="n">
         <v>25</v>
       </c>
-      <c r="K2" s="37" t="n">
+      <c r="K2" s="36" t="n">
         <v>25</v>
       </c>
-      <c r="L2" s="37" t="n">
+      <c r="L2" s="36" t="n">
         <v>25</v>
       </c>
-      <c r="M2" s="37" t="n">
+      <c r="M2" s="36" t="n">
         <v>25</v>
       </c>
-      <c r="N2" s="37" t="s">
+      <c r="N2" s="36" t="s">
         <v>160</v>
       </c>
-      <c r="O2" s="37" t="n">
-        <v>0</v>
-      </c>
-      <c r="P2" s="37" t="s">
+      <c r="O2" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="P2" s="36" t="s">
         <v>161</v>
       </c>
-      <c r="Q2" s="37" t="n">
+      <c r="Q2" s="36" t="n">
         <v>50</v>
       </c>
-      <c r="R2" s="37" t="s">
+      <c r="R2" s="36" t="s">
         <v>162</v>
       </c>
-      <c r="S2" s="37" t="n">
+      <c r="S2" s="36" t="n">
         <v>100</v>
       </c>
-      <c r="T2" s="37" t="s">
+      <c r="T2" s="36" t="s">
         <v>163</v>
       </c>
-      <c r="U2" s="37" t="s">
+      <c r="U2" s="36" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="37" t="s">
         <v>165</v>
       </c>
-      <c r="B3" s="37" t="n">
-        <v>0</v>
-      </c>
-      <c r="C3" s="37" t="n">
+      <c r="B3" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" s="36" t="n">
         <v>-50</v>
       </c>
-      <c r="D3" s="37" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" s="37" t="n">
+      <c r="D3" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="36" t="n">
         <v>-50</v>
       </c>
-      <c r="F3" s="37" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" s="37" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" s="37" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" s="37" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" s="37" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" s="37" t="n">
-        <v>0</v>
-      </c>
-      <c r="L3" s="37" t="n">
-        <v>0</v>
-      </c>
-      <c r="M3" s="37" t="n">
-        <v>0</v>
-      </c>
-      <c r="N3" s="37" t="n">
+      <c r="F3" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" s="36" t="n">
         <v>-50</v>
       </c>
-      <c r="O3" s="37" t="n">
+      <c r="O3" s="36" t="n">
         <v>-50</v>
       </c>
-      <c r="P3" s="37" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="37" t="n">
-        <v>0</v>
-      </c>
-      <c r="R3" s="37"/>
-      <c r="S3" s="37" t="n">
-        <v>0</v>
-      </c>
-      <c r="T3" s="37" t="n">
-        <v>0</v>
-      </c>
-      <c r="U3" s="37" t="n">
+      <c r="P3" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="R3" s="36"/>
+      <c r="S3" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="T3" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="U3" s="36" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="38" t="s">
         <v>166</v>
       </c>
-      <c r="B4" s="37" t="n">
+      <c r="B4" s="36" t="n">
         <v>50</v>
       </c>
-      <c r="C4" s="37" t="s">
+      <c r="C4" s="36" t="s">
         <v>167</v>
       </c>
-      <c r="D4" s="37" t="s">
+      <c r="D4" s="36" t="s">
         <v>168</v>
       </c>
-      <c r="E4" s="37" t="s">
+      <c r="E4" s="36" t="s">
         <v>169</v>
       </c>
-      <c r="F4" s="37" t="n">
+      <c r="F4" s="36" t="n">
         <v>50</v>
       </c>
-      <c r="G4" s="37" t="n">
+      <c r="G4" s="36" t="n">
         <v>50</v>
       </c>
-      <c r="H4" s="37" t="s">
+      <c r="H4" s="36" t="s">
         <v>164</v>
       </c>
-      <c r="I4" s="37" t="n">
+      <c r="I4" s="36" t="n">
         <v>50</v>
       </c>
-      <c r="J4" s="37" t="n">
+      <c r="J4" s="36" t="n">
         <v>50</v>
       </c>
-      <c r="K4" s="37" t="n">
+      <c r="K4" s="36" t="n">
         <v>50</v>
       </c>
-      <c r="L4" s="37" t="n">
+      <c r="L4" s="36" t="n">
         <v>50</v>
       </c>
-      <c r="M4" s="37" t="n">
+      <c r="M4" s="36" t="n">
         <v>50</v>
       </c>
-      <c r="N4" s="37" t="s">
+      <c r="N4" s="36" t="s">
         <v>170</v>
       </c>
-      <c r="O4" s="37" t="n">
+      <c r="O4" s="36" t="n">
         <v>50</v>
       </c>
-      <c r="P4" s="37" t="s">
+      <c r="P4" s="36" t="s">
         <v>164</v>
       </c>
-      <c r="Q4" s="37" t="n">
+      <c r="Q4" s="36" t="n">
         <v>50</v>
       </c>
-      <c r="R4" s="37" t="s">
+      <c r="R4" s="36" t="s">
         <v>170</v>
       </c>
-      <c r="S4" s="37" t="n">
+      <c r="S4" s="36" t="n">
         <v>50</v>
       </c>
-      <c r="T4" s="37" t="s">
+      <c r="T4" s="36" t="s">
         <v>164</v>
       </c>
-      <c r="U4" s="37" t="s">
+      <c r="U4" s="36" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="38" t="s">
         <v>171</v>
       </c>
-      <c r="B5" s="37" t="n">
-        <v>0</v>
-      </c>
-      <c r="C5" s="37" t="n">
+      <c r="B5" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="36" t="n">
         <v>-50</v>
       </c>
-      <c r="D5" s="37" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" s="37" t="n">
+      <c r="D5" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="36" t="n">
         <v>-50</v>
       </c>
-      <c r="F5" s="37" t="n">
+      <c r="F5" s="36" t="n">
         <v>-50</v>
       </c>
-      <c r="G5" s="37" t="n">
+      <c r="G5" s="36" t="n">
         <v>-50</v>
       </c>
-      <c r="H5" s="37" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" s="37" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" s="37" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" s="37" t="n">
-        <v>0</v>
-      </c>
-      <c r="L5" s="37" t="n">
-        <v>0</v>
-      </c>
-      <c r="M5" s="37" t="n">
-        <v>0</v>
-      </c>
-      <c r="N5" s="37" t="n">
+      <c r="H5" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" s="36" t="n">
         <v>-50</v>
       </c>
-      <c r="O5" s="37" t="n">
-        <v>0</v>
-      </c>
-      <c r="P5" s="37" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="37" t="n">
+      <c r="O5" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="36" t="n">
         <v>-50</v>
       </c>
-      <c r="R5" s="37"/>
-      <c r="S5" s="37" t="n">
-        <v>0</v>
-      </c>
-      <c r="T5" s="37" t="n">
-        <v>0</v>
-      </c>
-      <c r="U5" s="37" t="n">
+      <c r="R5" s="36"/>
+      <c r="S5" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="T5" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="U5" s="36" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="39" t="s">
         <v>172</v>
       </c>
-      <c r="B6" s="37" t="n">
+      <c r="B6" s="36" t="n">
         <v>0.75</v>
       </c>
-      <c r="C6" s="37" t="n">
+      <c r="C6" s="36" t="n">
         <v>0.75</v>
       </c>
-      <c r="D6" s="37" t="n">
+      <c r="D6" s="36" t="n">
         <v>0.75</v>
       </c>
-      <c r="E6" s="37" t="n">
+      <c r="E6" s="36" t="n">
         <v>0.75</v>
       </c>
-      <c r="F6" s="37" t="n">
+      <c r="F6" s="36" t="n">
         <v>0.75</v>
       </c>
-      <c r="G6" s="37" t="n">
+      <c r="G6" s="36" t="n">
         <v>0.75</v>
       </c>
-      <c r="H6" s="37" t="n">
+      <c r="H6" s="36" t="n">
         <v>1.25</v>
       </c>
-      <c r="I6" s="37" t="n">
+      <c r="I6" s="36" t="n">
         <v>1.5</v>
       </c>
-      <c r="J6" s="37" t="n">
+      <c r="J6" s="36" t="n">
         <v>1.5</v>
       </c>
-      <c r="K6" s="37" t="n">
+      <c r="K6" s="36" t="n">
         <v>1.5</v>
       </c>
-      <c r="L6" s="37" t="n">
+      <c r="L6" s="36" t="n">
         <v>1.5</v>
       </c>
-      <c r="M6" s="37" t="n">
+      <c r="M6" s="36" t="n">
         <v>1.5</v>
       </c>
-      <c r="N6" s="37" t="n">
+      <c r="N6" s="36" t="n">
         <v>1.5</v>
       </c>
-      <c r="O6" s="37" t="n">
+      <c r="O6" s="36" t="n">
         <v>1.5</v>
       </c>
-      <c r="P6" s="37" t="n">
+      <c r="P6" s="36" t="n">
         <v>1</v>
       </c>
-      <c r="Q6" s="37" t="n">
+      <c r="Q6" s="36" t="n">
         <v>0.75</v>
       </c>
-      <c r="R6" s="37" t="n">
+      <c r="R6" s="36" t="n">
         <v>0.75</v>
       </c>
-      <c r="S6" s="37" t="n">
+      <c r="S6" s="36" t="n">
         <v>0.75</v>
       </c>
-      <c r="T6" s="37" t="n">
+      <c r="T6" s="36" t="n">
         <v>0.75</v>
       </c>
-      <c r="U6" s="37" t="n">
+      <c r="U6" s="36" t="n">
         <v>0.75</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="41" t="s">
+      <c r="A7" s="40" t="s">
         <v>173</v>
       </c>
-      <c r="B7" s="37" t="n">
+      <c r="B7" s="36" t="n">
         <v>1.25</v>
       </c>
-      <c r="C7" s="37" t="n">
+      <c r="C7" s="36" t="n">
         <v>1.25</v>
       </c>
-      <c r="D7" s="37" t="n">
+      <c r="D7" s="36" t="n">
         <v>1.25</v>
       </c>
-      <c r="E7" s="37" t="n">
+      <c r="E7" s="36" t="n">
         <v>1.25</v>
       </c>
-      <c r="F7" s="37" t="n">
+      <c r="F7" s="36" t="n">
         <v>1.25</v>
       </c>
-      <c r="G7" s="37" t="n">
+      <c r="G7" s="36" t="n">
         <v>1.25</v>
       </c>
-      <c r="H7" s="37" t="n">
+      <c r="H7" s="36" t="n">
         <v>1.25</v>
       </c>
-      <c r="I7" s="37" t="n">
+      <c r="I7" s="36" t="n">
         <v>1.25</v>
       </c>
-      <c r="J7" s="37" t="n">
+      <c r="J7" s="36" t="n">
         <v>1.25</v>
       </c>
-      <c r="K7" s="37" t="n">
+      <c r="K7" s="36" t="n">
         <v>1.25</v>
       </c>
-      <c r="L7" s="37" t="n">
+      <c r="L7" s="36" t="n">
         <v>1.25</v>
       </c>
-      <c r="M7" s="37" t="n">
+      <c r="M7" s="36" t="n">
         <v>1.25</v>
       </c>
-      <c r="N7" s="37" t="n">
+      <c r="N7" s="36" t="n">
         <v>1.25</v>
       </c>
-      <c r="O7" s="37" t="n">
+      <c r="O7" s="36" t="n">
         <v>1.25</v>
       </c>
-      <c r="P7" s="37" t="n">
+      <c r="P7" s="36" t="n">
         <v>1.25</v>
       </c>
-      <c r="Q7" s="37" t="n">
+      <c r="Q7" s="36" t="n">
         <v>1.25</v>
       </c>
-      <c r="R7" s="37" t="n">
+      <c r="R7" s="36" t="n">
         <v>1.25</v>
       </c>
-      <c r="S7" s="37" t="n">
+      <c r="S7" s="36" t="n">
         <v>1.25</v>
       </c>
-      <c r="T7" s="37" t="n">
+      <c r="T7" s="36" t="n">
         <v>1.25</v>
       </c>
-      <c r="U7" s="37" t="n">
+      <c r="U7" s="36" t="n">
         <v>1.25</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="40" t="s">
         <v>174</v>
       </c>
-      <c r="B8" s="37" t="n">
+      <c r="B8" s="36" t="n">
         <v>1.5</v>
       </c>
-      <c r="C8" s="37" t="n">
+      <c r="C8" s="36" t="n">
         <v>1.5</v>
       </c>
-      <c r="D8" s="37" t="n">
+      <c r="D8" s="36" t="n">
         <v>1.5</v>
       </c>
-      <c r="E8" s="37" t="n">
+      <c r="E8" s="36" t="n">
         <v>1.5</v>
       </c>
-      <c r="F8" s="37" t="n">
+      <c r="F8" s="36" t="n">
         <v>1.5</v>
       </c>
-      <c r="G8" s="37" t="n">
+      <c r="G8" s="36" t="n">
         <v>1.5</v>
       </c>
-      <c r="H8" s="37" t="n">
+      <c r="H8" s="36" t="n">
         <v>1.5</v>
       </c>
-      <c r="I8" s="37" t="n">
+      <c r="I8" s="36" t="n">
         <v>1.5</v>
       </c>
-      <c r="J8" s="37" t="n">
+      <c r="J8" s="36" t="n">
         <v>1.5</v>
       </c>
-      <c r="K8" s="37" t="n">
+      <c r="K8" s="36" t="n">
         <v>1.5</v>
       </c>
-      <c r="L8" s="37" t="n">
+      <c r="L8" s="36" t="n">
         <v>1.5</v>
       </c>
-      <c r="M8" s="37" t="n">
+      <c r="M8" s="36" t="n">
         <v>1.5</v>
       </c>
-      <c r="N8" s="37" t="n">
+      <c r="N8" s="36" t="n">
         <v>1.5</v>
       </c>
-      <c r="O8" s="37" t="n">
+      <c r="O8" s="36" t="n">
         <v>1.5</v>
       </c>
-      <c r="P8" s="37" t="n">
+      <c r="P8" s="36" t="n">
         <v>1.5</v>
       </c>
-      <c r="Q8" s="37" t="n">
+      <c r="Q8" s="36" t="n">
         <v>1.5</v>
       </c>
-      <c r="R8" s="37" t="n">
+      <c r="R8" s="36" t="n">
         <v>1.5</v>
       </c>
-      <c r="S8" s="37" t="n">
+      <c r="S8" s="36" t="n">
         <v>1.5</v>
       </c>
-      <c r="T8" s="37" t="n">
+      <c r="T8" s="36" t="n">
         <v>1.5</v>
       </c>
-      <c r="U8" s="37" t="n">
+      <c r="U8" s="36" t="n">
         <v>1.5</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="42" t="s">
+      <c r="A9" s="41" t="s">
         <v>92</v>
       </c>
-      <c r="B9" s="37" t="n">
+      <c r="B9" s="36" t="n">
         <v>0.5</v>
       </c>
-      <c r="C9" s="37" t="n">
+      <c r="C9" s="36" t="n">
         <v>0.5</v>
       </c>
-      <c r="D9" s="37" t="n">
+      <c r="D9" s="36" t="n">
         <v>2</v>
       </c>
-      <c r="E9" s="37" t="n">
+      <c r="E9" s="36" t="n">
         <v>0.5</v>
       </c>
-      <c r="F9" s="37" t="n">
+      <c r="F9" s="36" t="n">
         <v>1</v>
       </c>
-      <c r="G9" s="37" t="n">
+      <c r="G9" s="36" t="n">
         <v>0.5</v>
       </c>
-      <c r="H9" s="37" t="n">
+      <c r="H9" s="36" t="n">
         <v>0.5</v>
       </c>
-      <c r="I9" s="37" t="n">
+      <c r="I9" s="36" t="n">
         <v>0.5</v>
       </c>
-      <c r="J9" s="37" t="n">
+      <c r="J9" s="36" t="n">
         <v>0.5</v>
       </c>
-      <c r="K9" s="37" t="n">
+      <c r="K9" s="36" t="n">
         <v>0.5</v>
       </c>
-      <c r="L9" s="37" t="n">
+      <c r="L9" s="36" t="n">
         <v>0.5</v>
       </c>
-      <c r="M9" s="37" t="n">
+      <c r="M9" s="36" t="n">
         <v>0.5</v>
       </c>
-      <c r="N9" s="37" t="n">
+      <c r="N9" s="36" t="n">
         <v>0.5</v>
       </c>
-      <c r="O9" s="37" t="n">
+      <c r="O9" s="36" t="n">
         <v>0.5</v>
       </c>
-      <c r="P9" s="37" t="n">
+      <c r="P9" s="36" t="n">
         <v>1</v>
       </c>
-      <c r="Q9" s="37" t="n">
+      <c r="Q9" s="36" t="n">
         <v>0.5</v>
       </c>
-      <c r="R9" s="37" t="n">
+      <c r="R9" s="36" t="n">
         <v>0.5</v>
       </c>
-      <c r="S9" s="37" t="n">
+      <c r="S9" s="36" t="n">
         <v>0.5</v>
       </c>
-      <c r="T9" s="37" t="n">
+      <c r="T9" s="36" t="n">
         <v>1</v>
       </c>
-      <c r="U9" s="37" t="n">
+      <c r="U9" s="36" t="n">
         <v>0.5</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="42" t="s">
+      <c r="A10" s="41" t="s">
         <v>109</v>
       </c>
-      <c r="B10" s="37" t="n">
+      <c r="B10" s="36" t="n">
         <v>0.75</v>
       </c>
-      <c r="C10" s="37" t="n">
+      <c r="C10" s="36" t="n">
         <v>0.75</v>
       </c>
-      <c r="D10" s="37" t="n">
+      <c r="D10" s="36" t="n">
         <v>1.5</v>
       </c>
-      <c r="E10" s="37" t="n">
+      <c r="E10" s="36" t="n">
         <v>0.75</v>
       </c>
-      <c r="F10" s="37" t="n">
+      <c r="F10" s="36" t="n">
         <v>1</v>
       </c>
-      <c r="G10" s="37" t="n">
+      <c r="G10" s="36" t="n">
         <v>0.75</v>
       </c>
-      <c r="H10" s="37" t="n">
+      <c r="H10" s="36" t="n">
         <v>0.75</v>
       </c>
-      <c r="I10" s="37" t="n">
+      <c r="I10" s="36" t="n">
         <v>0.75</v>
       </c>
-      <c r="J10" s="37" t="n">
+      <c r="J10" s="36" t="n">
         <v>0.75</v>
       </c>
-      <c r="K10" s="37" t="n">
+      <c r="K10" s="36" t="n">
         <v>0.75</v>
       </c>
-      <c r="L10" s="37" t="n">
+      <c r="L10" s="36" t="n">
         <v>0.75</v>
       </c>
-      <c r="M10" s="37" t="n">
+      <c r="M10" s="36" t="n">
         <v>0.75</v>
       </c>
-      <c r="N10" s="37" t="n">
+      <c r="N10" s="36" t="n">
         <v>0.75</v>
       </c>
-      <c r="O10" s="37" t="n">
+      <c r="O10" s="36" t="n">
         <v>0.75</v>
       </c>
-      <c r="P10" s="37" t="n">
+      <c r="P10" s="36" t="n">
         <v>1</v>
       </c>
-      <c r="Q10" s="37" t="n">
+      <c r="Q10" s="36" t="n">
         <v>0.75</v>
       </c>
-      <c r="R10" s="37" t="n">
+      <c r="R10" s="36" t="n">
         <v>0.75</v>
       </c>
-      <c r="S10" s="37" t="n">
+      <c r="S10" s="36" t="n">
         <v>0.75</v>
       </c>
-      <c r="T10" s="37" t="n">
+      <c r="T10" s="36" t="n">
         <v>1</v>
       </c>
-      <c r="U10" s="37" t="n">
+      <c r="U10" s="36" t="n">
         <v>0.75</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="43" t="s">
+      <c r="A11" s="42" t="s">
         <v>175</v>
       </c>
-      <c r="B11" s="37" t="n">
+      <c r="B11" s="36" t="n">
         <v>1</v>
       </c>
-      <c r="C11" s="37" t="n">
+      <c r="C11" s="36" t="n">
         <v>1</v>
       </c>
-      <c r="D11" s="37" t="n">
+      <c r="D11" s="36" t="n">
         <v>1</v>
       </c>
-      <c r="E11" s="37" t="n">
+      <c r="E11" s="36" t="n">
         <v>1</v>
       </c>
-      <c r="F11" s="37" t="n">
+      <c r="F11" s="36" t="n">
         <v>1</v>
       </c>
-      <c r="G11" s="37" t="s">
+      <c r="G11" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="H11" s="37" t="n">
+      <c r="H11" s="36" t="n">
         <v>1</v>
       </c>
-      <c r="I11" s="37" t="n">
+      <c r="I11" s="36" t="n">
         <v>1</v>
       </c>
-      <c r="J11" s="37" t="s">
+      <c r="J11" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="K11" s="37" t="s">
+      <c r="K11" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="L11" s="37" t="s">
+      <c r="L11" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="M11" s="37" t="s">
+      <c r="M11" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="N11" s="37" t="s">
+      <c r="N11" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="O11" s="37" t="s">
+      <c r="O11" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="P11" s="37" t="n">
+      <c r="P11" s="36" t="n">
         <v>1</v>
       </c>
-      <c r="Q11" s="37" t="n">
+      <c r="Q11" s="36" t="n">
         <v>1</v>
       </c>
-      <c r="R11" s="37" t="n">
+      <c r="R11" s="36" t="n">
         <v>1</v>
       </c>
-      <c r="S11" s="37" t="s">
+      <c r="S11" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="T11" s="37" t="n">
+      <c r="T11" s="36" t="n">
         <v>1.5</v>
       </c>
-      <c r="U11" s="37" t="n">
+      <c r="U11" s="36" t="n">
         <v>1</v>
       </c>
     </row>
@@ -6372,7 +6367,7 @@
       <selection pane="topLeft" activeCell="K6" activeCellId="0" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="31" width="9.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="31" width="5.43"/>
@@ -6389,7 +6384,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="31" width="7.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="11.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="31" width="6.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="19" style="31" width="7.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="19" style="31" width="7.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="11.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="31" width="6.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="23" style="31" width="9.14"/>
@@ -6722,48 +6717,48 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F8" s="44"/>
-      <c r="H8" s="44"/>
+      <c r="F8" s="43"/>
+      <c r="H8" s="43"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F9" s="44"/>
-      <c r="H9" s="44"/>
+      <c r="F9" s="43"/>
+      <c r="H9" s="43"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F10" s="44"/>
-      <c r="H10" s="44"/>
+      <c r="F10" s="43"/>
+      <c r="H10" s="43"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F11" s="44"/>
-      <c r="H11" s="44"/>
+      <c r="F11" s="43"/>
+      <c r="H11" s="43"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F12" s="44"/>
-      <c r="H12" s="44"/>
+      <c r="F12" s="43"/>
+      <c r="H12" s="43"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F13" s="44"/>
-      <c r="H13" s="44"/>
+      <c r="F13" s="43"/>
+      <c r="H13" s="43"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F14" s="44"/>
-      <c r="H14" s="44"/>
+      <c r="F14" s="43"/>
+      <c r="H14" s="43"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F15" s="44"/>
-      <c r="H15" s="44"/>
+      <c r="F15" s="43"/>
+      <c r="H15" s="43"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F16" s="44"/>
-      <c r="H16" s="44"/>
+      <c r="F16" s="43"/>
+      <c r="H16" s="43"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F17" s="44"/>
-      <c r="H17" s="44"/>
+      <c r="F17" s="43"/>
+      <c r="H17" s="43"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F18" s="44"/>
-      <c r="H18" s="44"/>
+      <c r="F18" s="43"/>
+      <c r="H18" s="43"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>